<commit_message>
Ajout de mon pour la partie 1
</commit_message>
<xml_diff>
--- a/Rapport_Reel_TP2.xlsx
+++ b/Rapport_Reel_TP2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LordCatzorz\Documents\GLO-2001-TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA715B61-70A2-406A-A7D9-4AAFDC26125E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A22C61-B8E3-4647-A768-AC0194555567}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -973,8 +973,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:S94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1042,9 @@
       <c r="C9" s="11">
         <v>2</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="11">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -1054,7 +1056,9 @@
       <c r="C10" s="11">
         <v>0.25</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1066,7 +1070,9 @@
       <c r="C11" s="11">
         <v>0.25</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
@@ -1078,7 +1084,9 @@
       <c r="C12" s="11">
         <v>0.25</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
@@ -1090,7 +1098,9 @@
       <c r="C13" s="11">
         <v>0.25</v>
       </c>
-      <c r="D13" s="11"/>
+      <c r="D13" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -1102,7 +1112,9 @@
       <c r="C14" s="11">
         <v>0.25</v>
       </c>
-      <c r="D14" s="11"/>
+      <c r="D14" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -1114,7 +1126,9 @@
       <c r="C15" s="11">
         <v>1.5</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="11">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
@@ -1356,7 +1370,9 @@
       <c r="C36" s="11">
         <v>3</v>
       </c>
-      <c r="D36" s="11"/>
+      <c r="D36" s="11">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
@@ -1387,7 +1403,7 @@
       </c>
       <c r="D40" s="6">
         <f>SUM(D8:D39)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1396,9 +1412,9 @@
         <v>5</v>
       </c>
       <c r="C41" s="4"/>
-      <c r="D41" s="4" t="e">
+      <c r="D41" s="4">
         <f>IF(C40&lt;&gt;0,D40/SUMIF(D8:D39,"&gt;0",C8:C39),0)</f>
-        <v>#DIV/0!</v>
+        <v>0.15384615384615385</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ajout de mon temps rapport preliminaire
</commit_message>
<xml_diff>
--- a/Rapport_Reel_TP2.xlsx
+++ b/Rapport_Reel_TP2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LordCatzorz\Documents\GLO-2001-TP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maximeprieur/GLO-2001-TP2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA715B61-70A2-406A-A7D9-4AAFDC26125E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58D1F41-EA57-7D46-A89B-9DBC44C94C2B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2680" yWindow="2680" windowWidth="21600" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -266,7 +260,7 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -540,16 +534,16 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -664,10 +658,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -973,34 +967,34 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:S94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="63.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="18" max="18" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="63.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
@@ -1008,7 +1002,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
@@ -1032,7 +1026,7 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
@@ -1042,9 +1036,11 @@
       <c r="C9" s="11">
         <v>2</v>
       </c>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>12</v>
       </c>
@@ -1054,9 +1050,11 @@
       <c r="C10" s="11">
         <v>0.25</v>
       </c>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="11">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
@@ -1066,9 +1064,11 @@
       <c r="C11" s="11">
         <v>0.25</v>
       </c>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="11">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>14</v>
       </c>
@@ -1078,9 +1078,11 @@
       <c r="C12" s="11">
         <v>0.25</v>
       </c>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="11">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -1090,9 +1092,11 @@
       <c r="C13" s="11">
         <v>0.25</v>
       </c>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="11">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>16</v>
       </c>
@@ -1102,9 +1106,11 @@
       <c r="C14" s="11">
         <v>0.25</v>
       </c>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D14" s="11">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
@@ -1114,9 +1120,11 @@
       <c r="C15" s="11">
         <v>1.5</v>
       </c>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
@@ -1126,9 +1134,11 @@
       <c r="C16" s="11">
         <v>2</v>
       </c>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="11">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>2</v>
       </c>
@@ -1136,9 +1146,11 @@
         <v>19</v>
       </c>
       <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="11">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>20</v>
       </c>
@@ -1150,7 +1162,7 @@
       </c>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>22</v>
       </c>
@@ -1162,7 +1174,7 @@
       </c>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -1174,7 +1186,7 @@
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>26</v>
       </c>
@@ -1186,7 +1198,7 @@
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>27</v>
       </c>
@@ -1198,7 +1210,7 @@
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>28</v>
       </c>
@@ -1210,7 +1222,7 @@
       </c>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>29</v>
       </c>
@@ -1222,7 +1234,7 @@
       </c>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>30</v>
       </c>
@@ -1234,7 +1246,7 @@
       </c>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>3</v>
       </c>
@@ -1244,7 +1256,7 @@
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>32</v>
       </c>
@@ -1256,7 +1268,7 @@
       </c>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>34</v>
       </c>
@@ -1268,7 +1280,7 @@
       </c>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>36</v>
       </c>
@@ -1280,7 +1292,7 @@
       </c>
       <c r="D29" s="11"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>38</v>
       </c>
@@ -1292,7 +1304,7 @@
       </c>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>39</v>
       </c>
@@ -1304,7 +1316,7 @@
       </c>
       <c r="D31" s="11"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>40</v>
       </c>
@@ -1316,7 +1328,7 @@
       </c>
       <c r="D32" s="11"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>41</v>
       </c>
@@ -1328,7 +1340,7 @@
       </c>
       <c r="D33" s="11"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>42</v>
       </c>
@@ -1340,13 +1352,13 @@
       </c>
       <c r="D34" s="11"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>63</v>
       </c>
@@ -1358,25 +1370,25 @@
       </c>
       <c r="D36" s="11"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
     </row>
-    <row r="40" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
       <c r="B40" s="7" t="s">
         <v>4</v>
@@ -1387,258 +1399,258 @@
       </c>
       <c r="D40" s="6">
         <f>SUM(D8:D39)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="4"/>
-      <c r="D41" s="4" t="e">
+      <c r="D41" s="4">
         <f>IF(C40&lt;&gt;0,D40/SUMIF(D8:D39,"&gt;0",C8:C39),0)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.5185185185185186</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
     </row>
-    <row r="49" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S53">
         <v>0.125</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S54">
         <v>0.25</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S55">
         <v>0.375</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S56">
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S57">
         <v>0.625</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S58">
         <v>0.75</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S59">
         <v>0.875</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S61">
         <v>1.25</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S62">
         <v>1.5</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S63">
         <v>1.75</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="S64">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S65">
         <v>2.25</v>
       </c>
     </row>
-    <row r="66" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S66">
         <v>2.5</v>
       </c>
     </row>
-    <row r="67" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S67">
         <v>2.75</v>
       </c>
     </row>
-    <row r="68" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S68">
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S69">
         <v>3.25</v>
       </c>
     </row>
-    <row r="70" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S70">
         <v>3.5</v>
       </c>
     </row>
-    <row r="71" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S71">
         <v>3.75</v>
       </c>
     </row>
-    <row r="72" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S72">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S73">
         <v>4.25</v>
       </c>
     </row>
-    <row r="74" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S74">
         <v>4.5</v>
       </c>
     </row>
-    <row r="75" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S75">
         <v>4.75</v>
       </c>
     </row>
-    <row r="76" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S76">
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S77">
         <v>5.25</v>
       </c>
     </row>
-    <row r="78" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S78">
         <v>5.5</v>
       </c>
     </row>
-    <row r="79" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S79">
         <v>5.75</v>
       </c>
     </row>
-    <row r="80" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S80">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S81">
         <v>6.25</v>
       </c>
     </row>
-    <row r="82" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S82">
         <v>6.5</v>
       </c>
     </row>
-    <row r="83" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S83">
         <v>6.75</v>
       </c>
     </row>
-    <row r="84" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S84">
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S85">
         <v>7.25</v>
       </c>
     </row>
-    <row r="86" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S86">
         <v>7.5</v>
       </c>
     </row>
-    <row r="87" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S87">
         <v>7.75</v>
       </c>
     </row>
-    <row r="88" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S88">
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S89">
         <v>8.25</v>
       </c>
     </row>
-    <row r="90" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S90">
         <v>8.5</v>
       </c>
     </row>
-    <row r="91" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S91">
         <v>8.75</v>
       </c>
     </row>
-    <row r="92" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S92">
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S93">
         <v>9.25</v>
       </c>
     </row>
-    <row r="94" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S94">
         <v>9.5</v>
       </c>
@@ -1663,7 +1675,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1676,7 +1688,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout temps pour fifo
</commit_message>
<xml_diff>
--- a/Rapport_Reel_TP2.xlsx
+++ b/Rapport_Reel_TP2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LordCatzorz\Documents\GLO-2001-TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A22C61-B8E3-4647-A768-AC0194555567}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A9FC63-4BD9-4B6C-AC0D-ED5B4A6B2DDE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -279,7 +279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>No</t>
   </si>
@@ -474,6 +474,9 @@
   </si>
   <si>
     <t>Correction / Révision / Formattage / Packaging</t>
+  </si>
+  <si>
+    <t>fifo 1</t>
   </si>
 </sst>
 </file>
@@ -973,8 +976,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:S94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,22 +988,22 @@
     <col min="18" max="18" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
@@ -1032,7 +1035,7 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>12</v>
       </c>
@@ -1060,7 +1063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
@@ -1074,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>14</v>
       </c>
@@ -1088,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>16</v>
       </c>
@@ -1116,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
@@ -1130,7 +1133,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
@@ -1141,6 +1144,9 @@
         <v>2</v>
       </c>
       <c r="D16" s="11"/>
+      <c r="E16" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="11">

</xml_diff>